<commit_message>
Updated School_Data & School_Data_Beta
</commit_message>
<xml_diff>
--- a/resources/app/School_Data.xlsx
+++ b/resources/app/School_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahngu\Desktop\ncaa-ps2-scheduler-ui-win32-x64\resources\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\NCAA-PS2-Scheduler-UI\resources\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC238E4-737D-4CDA-B0DC-EA38040EB856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2969168-4CDC-4630-A763-96C66AC67947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="930" windowWidth="23535" windowHeight="18525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="704">
   <si>
     <t>TGID</t>
   </si>
@@ -2110,6 +2110,36 @@
   </si>
   <si>
     <t>Golden Panthers</t>
+  </si>
+  <si>
+    <t>1AA East</t>
+  </si>
+  <si>
+    <t>1AA Midwest</t>
+  </si>
+  <si>
+    <t>1AA Northwest</t>
+  </si>
+  <si>
+    <t>1AA Southeast</t>
+  </si>
+  <si>
+    <t>1AA West</t>
+  </si>
+  <si>
+    <t>1AAE</t>
+  </si>
+  <si>
+    <t>1AAW</t>
+  </si>
+  <si>
+    <t>1AANW</t>
+  </si>
+  <si>
+    <t>1AAMW</t>
+  </si>
+  <si>
+    <t>1AASE</t>
   </si>
 </sst>
 </file>
@@ -2623,8 +2653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB1121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="G169" sqref="G169"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="G206" sqref="G206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16703,9 +16733,15 @@
       <c r="BA196" s="5"/>
     </row>
     <row r="197" spans="1:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="5"/>
-      <c r="B197" s="5"/>
-      <c r="C197" s="5"/>
+      <c r="A197" s="5">
+        <v>160</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="C197" s="5" t="s">
+        <v>699</v>
+      </c>
       <c r="D197" s="5"/>
       <c r="E197" s="5"/>
       <c r="F197" s="5"/>
@@ -16758,9 +16794,15 @@
       <c r="BA197" s="5"/>
     </row>
     <row r="198" spans="1:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="5"/>
-      <c r="B198" s="5"/>
-      <c r="C198" s="5"/>
+      <c r="A198" s="5">
+        <v>163</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>702</v>
+      </c>
       <c r="D198" s="5"/>
       <c r="E198" s="5"/>
       <c r="F198" s="5"/>
@@ -16813,9 +16855,15 @@
       <c r="BA198" s="5"/>
     </row>
     <row r="199" spans="1:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A199" s="5"/>
-      <c r="B199" s="5"/>
-      <c r="C199" s="5"/>
+      <c r="A199" s="5">
+        <v>162</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="C199" s="5" t="s">
+        <v>701</v>
+      </c>
       <c r="D199" s="5"/>
       <c r="E199" s="5"/>
       <c r="F199" s="5"/>
@@ -16868,9 +16916,15 @@
       <c r="BA199" s="5"/>
     </row>
     <row r="200" spans="1:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A200" s="5"/>
-      <c r="B200" s="5"/>
-      <c r="C200" s="5"/>
+      <c r="A200" s="5">
+        <v>164</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>703</v>
+      </c>
       <c r="D200" s="5"/>
       <c r="E200" s="5"/>
       <c r="F200" s="5"/>
@@ -16923,9 +16977,15 @@
       <c r="BA200" s="5"/>
     </row>
     <row r="201" spans="1:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A201" s="5"/>
-      <c r="B201" s="5"/>
-      <c r="C201" s="5"/>
+      <c r="A201" s="5">
+        <v>161</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="C201" s="5" t="s">
+        <v>700</v>
+      </c>
       <c r="D201" s="5"/>
       <c r="E201" s="5"/>
       <c r="F201" s="5"/>

</xml_diff>